<commit_message>
test-18: new exp for 3mig hybrid
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-18.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-18.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="mae" sheetId="1" r:id="rId1"/>
     <sheet name="mse" sheetId="2" r:id="rId2"/>
+    <sheet name="r2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="12">
   <si>
     <t>Random Forest-100 (superdataset-24.csv)</t>
   </si>
@@ -50,6 +51,12 @@
   </si>
   <si>
     <t>Hybrid 3mig (superdataset-24 3mig.csv) test 0.2%</t>
+  </si>
+  <si>
+    <t>train (R2)</t>
+  </si>
+  <si>
+    <t>test (R2)</t>
   </si>
 </sst>
 </file>
@@ -404,8 +411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:T58"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:E58"/>
+    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I60" sqref="I60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2301,8 +2308,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D4:Z58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H34" workbookViewId="0">
-      <selection activeCell="AA49" sqref="AA49"/>
+    <sheetView topLeftCell="H25" workbookViewId="0">
+      <selection activeCell="X59" sqref="X59:X60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5097,4 +5104,663 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C4:E58"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.91674965606328518</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.41865481479112993</v>
+      </c>
+    </row>
+    <row r="7" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C7" s="2">
+        <f>C6+1</f>
+        <v>2</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.91662836413391258</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.41210315792372543</v>
+      </c>
+    </row>
+    <row r="8" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C8" s="2">
+        <f t="shared" ref="C8:C55" si="0">C7+1</f>
+        <v>3</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.91489374854208771</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.37349382585140262</v>
+      </c>
+    </row>
+    <row r="9" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C9" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.9179718452745893</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.36497913160234158</v>
+      </c>
+    </row>
+    <row r="10" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C10" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.91749802011473403</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.35425807036740548</v>
+      </c>
+    </row>
+    <row r="11" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C11" s="2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0.91521027682556311</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0.42320774970929909</v>
+      </c>
+    </row>
+    <row r="12" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C12" s="2">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.91500589062971482</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.41681088493508539</v>
+      </c>
+    </row>
+    <row r="13" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C13" s="2">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0.91798473101443356</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0.38346122783214492</v>
+      </c>
+    </row>
+    <row r="14" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C14" s="2">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0.91719097345680278</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0.39056416952125128</v>
+      </c>
+    </row>
+    <row r="15" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C15" s="2">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0.91587940697306547</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0.37845940890745139</v>
+      </c>
+    </row>
+    <row r="16" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C16" s="2">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0.91660470785204606</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0.4291801637251399</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C17" s="2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0.91258083463588713</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0.44705496932774619</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C18" s="2">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0.91929141987271945</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0.35528633728632808</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C19" s="2">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0.91446787102524096</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0.4550027743195163</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C20" s="2">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="D20" s="3">
+        <v>0.91454986537073446</v>
+      </c>
+      <c r="E20" s="3">
+        <v>0.4140300140183707</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C21" s="2">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0.91376073747995268</v>
+      </c>
+      <c r="E21" s="3">
+        <v>0.43169068986400971</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C22" s="2">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0.91518188406348921</v>
+      </c>
+      <c r="E22" s="3">
+        <v>0.40094238655350939</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C23" s="2">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0.91493019291344302</v>
+      </c>
+      <c r="E23" s="3">
+        <v>0.39267919439608012</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C24" s="2">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="D24" s="3">
+        <v>0.91563121732443498</v>
+      </c>
+      <c r="E24" s="3">
+        <v>0.38572013805779343</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C25" s="2">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="D25" s="3">
+        <v>0.91773165442710813</v>
+      </c>
+      <c r="E25" s="3">
+        <v>0.38473101368170481</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C26" s="2">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="D26" s="3">
+        <v>0.9177091603404175</v>
+      </c>
+      <c r="E26" s="3">
+        <v>0.37480854878139552</v>
+      </c>
+    </row>
+    <row r="27" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C27" s="2">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="D27" s="3">
+        <v>0.91497542739021487</v>
+      </c>
+      <c r="E27" s="3">
+        <v>0.40341346598812078</v>
+      </c>
+    </row>
+    <row r="28" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C28" s="2">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="D28" s="3">
+        <v>0.91288243481060105</v>
+      </c>
+      <c r="E28" s="3">
+        <v>0.42614942460100058</v>
+      </c>
+    </row>
+    <row r="29" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C29" s="2">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="D29" s="3">
+        <v>0.91725644299011833</v>
+      </c>
+      <c r="E29" s="3">
+        <v>0.39629742607011359</v>
+      </c>
+    </row>
+    <row r="30" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C30" s="2">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="D30" s="3">
+        <v>0.9148759539994844</v>
+      </c>
+      <c r="E30" s="3">
+        <v>0.4502914764564756</v>
+      </c>
+    </row>
+    <row r="31" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C31" s="2">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="D31" s="3">
+        <v>0.91678622769515294</v>
+      </c>
+      <c r="E31" s="3">
+        <v>0.38842104967516289</v>
+      </c>
+    </row>
+    <row r="32" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C32" s="2">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="D32" s="3">
+        <v>0.91466036529433836</v>
+      </c>
+      <c r="E32" s="3">
+        <v>0.39157194431333242</v>
+      </c>
+    </row>
+    <row r="33" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C33" s="2">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="D33" s="3">
+        <v>0.91718669404871811</v>
+      </c>
+      <c r="E33" s="3">
+        <v>0.40554870539091431</v>
+      </c>
+    </row>
+    <row r="34" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C34" s="2">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="D34" s="3">
+        <v>0.9132905690155908</v>
+      </c>
+      <c r="E34" s="3">
+        <v>0.42285303533815077</v>
+      </c>
+    </row>
+    <row r="35" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C35" s="2">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="D35" s="3">
+        <v>0.91575489294291046</v>
+      </c>
+      <c r="E35" s="3">
+        <v>0.37645344715615092</v>
+      </c>
+    </row>
+    <row r="36" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C36" s="2">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="D36" s="3">
+        <v>0.91795557567381492</v>
+      </c>
+      <c r="E36" s="3">
+        <v>0.36772915212961871</v>
+      </c>
+    </row>
+    <row r="37" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C37" s="2">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="D37" s="3">
+        <v>0.91510660905137842</v>
+      </c>
+      <c r="E37" s="3">
+        <v>0.38995263407565273</v>
+      </c>
+    </row>
+    <row r="38" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C38" s="2">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="D38" s="3">
+        <v>0.91576625669633493</v>
+      </c>
+      <c r="E38" s="3">
+        <v>0.39959890054089942</v>
+      </c>
+    </row>
+    <row r="39" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C39" s="2">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="D39" s="3">
+        <v>0.91209299014335043</v>
+      </c>
+      <c r="E39" s="3">
+        <v>0.45364619716090399</v>
+      </c>
+    </row>
+    <row r="40" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C40" s="2">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="D40" s="3">
+        <v>0.91701078366971889</v>
+      </c>
+      <c r="E40" s="3">
+        <v>0.39197471705611298</v>
+      </c>
+    </row>
+    <row r="41" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C41" s="2">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="D41" s="3">
+        <v>0.91597329151734264</v>
+      </c>
+      <c r="E41" s="3">
+        <v>0.3668016480528129</v>
+      </c>
+    </row>
+    <row r="42" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C42" s="2">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="D42" s="3">
+        <v>0.91512740825651906</v>
+      </c>
+      <c r="E42" s="3">
+        <v>0.39628461256361852</v>
+      </c>
+    </row>
+    <row r="43" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C43" s="2">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="D43" s="3">
+        <v>0.91473923728198114</v>
+      </c>
+      <c r="E43" s="3">
+        <v>0.41515535442898149</v>
+      </c>
+    </row>
+    <row r="44" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C44" s="2">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="D44" s="3">
+        <v>0.92016495157705191</v>
+      </c>
+      <c r="E44" s="3">
+        <v>0.2998262978905829</v>
+      </c>
+    </row>
+    <row r="45" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C45" s="2">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="D45" s="3">
+        <v>0.91482996105848169</v>
+      </c>
+      <c r="E45" s="3">
+        <v>0.40981672540456071</v>
+      </c>
+    </row>
+    <row r="46" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C46" s="2">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="D46" s="3">
+        <v>0.91746710160711187</v>
+      </c>
+      <c r="E46" s="3">
+        <v>0.3647611651907382</v>
+      </c>
+    </row>
+    <row r="47" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C47" s="2">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="D47" s="3">
+        <v>0.91520760190949124</v>
+      </c>
+      <c r="E47" s="3">
+        <v>0.41982998640320562</v>
+      </c>
+    </row>
+    <row r="48" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C48" s="2">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="D48" s="3">
+        <v>0.91665084412482056</v>
+      </c>
+      <c r="E48" s="3">
+        <v>0.3680528717488325</v>
+      </c>
+    </row>
+    <row r="49" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C49" s="2">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="D49" s="3">
+        <v>0.91493635664586281</v>
+      </c>
+      <c r="E49" s="3">
+        <v>0.42906569543776218</v>
+      </c>
+    </row>
+    <row r="50" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C50" s="2">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="D50" s="3">
+        <v>0.91546809558539488</v>
+      </c>
+      <c r="E50" s="3">
+        <v>0.41725197036721878</v>
+      </c>
+    </row>
+    <row r="51" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C51" s="2">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="D51" s="3">
+        <v>0.9145235748615701</v>
+      </c>
+      <c r="E51" s="3">
+        <v>0.39860229396178121</v>
+      </c>
+    </row>
+    <row r="52" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C52" s="2">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D52" s="3">
+        <v>0.91822709537347291</v>
+      </c>
+      <c r="E52" s="3">
+        <v>0.3811138190167358</v>
+      </c>
+    </row>
+    <row r="53" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C53" s="2">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="D53" s="3">
+        <v>0.91658804181314613</v>
+      </c>
+      <c r="E53" s="3">
+        <v>0.35460928371796668</v>
+      </c>
+    </row>
+    <row r="54" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C54" s="2">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="D54" s="3">
+        <v>0.91607303013344088</v>
+      </c>
+      <c r="E54" s="3">
+        <v>0.39728715348673588</v>
+      </c>
+    </row>
+    <row r="55" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C55" s="2">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="D55" s="3">
+        <v>0.91815368464161695</v>
+      </c>
+      <c r="E55" s="3">
+        <v>0.37763994819718932</v>
+      </c>
+    </row>
+    <row r="57" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C57" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D57" s="3">
+        <f>AVERAGE(D6:D55)</f>
+        <v>0.91594367916285369</v>
+      </c>
+      <c r="E57" s="3">
+        <f>AVERAGE(E6:E55)</f>
+        <v>0.39694238146548327</v>
+      </c>
+    </row>
+    <row r="58" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C58" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D58" s="3">
+        <f>_xlfn.STDEV.S(D6:D55)</f>
+        <v>1.6841027687637684E-3</v>
+      </c>
+      <c r="E58" s="3">
+        <f>_xlfn.STDEV.S(E6:E55)</f>
+        <v>2.9606486921015984E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
upd. test-18 (3mig size of 2Y)
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-18.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-18.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="15">
   <si>
     <t>Random Forest-100 (superdataset-24.csv)</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>Random Forest-100 (superdataset-24 3mig 2Y.csv)</t>
+  </si>
+  <si>
+    <t>RF-100 (superdataset-24 3mig.csv) size of 2Y</t>
   </si>
 </sst>
 </file>
@@ -417,7 +420,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:T58"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="I60" sqref="I60"/>
     </sheetView>
   </sheetViews>
@@ -2314,7 +2317,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D4:Z58"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="X59" sqref="X59:X60"/>
     </sheetView>
   </sheetViews>
@@ -5114,10 +5117,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4:O58"/>
+  <dimension ref="C4:T58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S34" sqref="S34"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="W37" sqref="W37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5126,7 +5129,7 @@
     <col min="5" max="5" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
@@ -5136,11 +5139,15 @@
       </c>
       <c r="J4" s="1"/>
       <c r="M4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O4" s="1"/>
+      <c r="R4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O4" s="1"/>
-    </row>
-    <row r="5" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="T4" s="1"/>
+    </row>
+    <row r="5" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
         <v>10</v>
@@ -5162,8 +5169,15 @@
       <c r="O5" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="R5" s="2"/>
+      <c r="S5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C6" s="2">
         <v>1</v>
       </c>
@@ -5186,13 +5200,22 @@
         <v>1</v>
       </c>
       <c r="N6" s="3">
+        <v>0.91340869996178564</v>
+      </c>
+      <c r="O6" s="3">
+        <v>0.35962953778405538</v>
+      </c>
+      <c r="R6" s="2">
+        <v>1</v>
+      </c>
+      <c r="S6" s="3">
         <v>0.91484594607381897</v>
       </c>
-      <c r="O6" s="3">
+      <c r="T6" s="3">
         <v>0.40331810439083332</v>
       </c>
     </row>
-    <row r="7" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C7" s="2">
         <f>C6+1</f>
         <v>2</v>
@@ -5218,13 +5241,23 @@
         <v>2</v>
       </c>
       <c r="N7" s="3">
+        <v>0.91412736713647624</v>
+      </c>
+      <c r="O7" s="3">
+        <v>0.31130414951001822</v>
+      </c>
+      <c r="R7" s="2">
+        <f>R6+1</f>
+        <v>2</v>
+      </c>
+      <c r="S7" s="3">
         <v>0.91667794975123895</v>
       </c>
-      <c r="O7" s="3">
+      <c r="T7" s="3">
         <v>0.43020733919834531</v>
       </c>
     </row>
-    <row r="8" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C8" s="2">
         <f t="shared" ref="C8:C55" si="0">C7+1</f>
         <v>3</v>
@@ -5250,13 +5283,23 @@
         <v>3</v>
       </c>
       <c r="N8" s="3">
+        <v>0.90912875757528377</v>
+      </c>
+      <c r="O8" s="3">
+        <v>0.45885034479721171</v>
+      </c>
+      <c r="R8" s="2">
+        <f t="shared" ref="R8:R55" si="3">R7+1</f>
+        <v>3</v>
+      </c>
+      <c r="S8" s="3">
         <v>0.91571373111051513</v>
       </c>
-      <c r="O8" s="3">
+      <c r="T8" s="3">
         <v>0.41061397673470079</v>
       </c>
     </row>
-    <row r="9" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C9" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -5282,13 +5325,23 @@
         <v>4</v>
       </c>
       <c r="N9" s="3">
+        <v>0.91565542971313596</v>
+      </c>
+      <c r="O9" s="3">
+        <v>0.33633265761295328</v>
+      </c>
+      <c r="R9" s="2">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="S9" s="3">
         <v>0.91396390107515846</v>
       </c>
-      <c r="O9" s="3">
+      <c r="T9" s="3">
         <v>0.41138880396830019</v>
       </c>
     </row>
-    <row r="10" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C10" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -5314,13 +5367,23 @@
         <v>5</v>
       </c>
       <c r="N10" s="3">
+        <v>0.91650190013630728</v>
+      </c>
+      <c r="O10" s="3">
+        <v>0.35528296420754468</v>
+      </c>
+      <c r="R10" s="2">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="S10" s="3">
         <v>0.91477552297645726</v>
       </c>
-      <c r="O10" s="3">
+      <c r="T10" s="3">
         <v>0.42060480731108701</v>
       </c>
     </row>
-    <row r="11" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C11" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -5346,13 +5409,23 @@
         <v>6</v>
       </c>
       <c r="N11" s="3">
+        <v>0.91419308732927684</v>
+      </c>
+      <c r="O11" s="3">
+        <v>0.35943153817061407</v>
+      </c>
+      <c r="R11" s="2">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="S11" s="3">
         <v>0.91382568808394726</v>
       </c>
-      <c r="O11" s="3">
+      <c r="T11" s="3">
         <v>0.4211635870948931</v>
       </c>
     </row>
-    <row r="12" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C12" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -5378,13 +5451,23 @@
         <v>7</v>
       </c>
       <c r="N12" s="3">
+        <v>0.91068169101902174</v>
+      </c>
+      <c r="O12" s="3">
+        <v>0.37601163446220037</v>
+      </c>
+      <c r="R12" s="2">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="S12" s="3">
         <v>0.91678753156962245</v>
       </c>
-      <c r="O12" s="3">
+      <c r="T12" s="3">
         <v>0.40076581070785361</v>
       </c>
     </row>
-    <row r="13" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C13" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -5410,13 +5493,23 @@
         <v>8</v>
       </c>
       <c r="N13" s="3">
+        <v>0.91043310950570444</v>
+      </c>
+      <c r="O13" s="3">
+        <v>0.41630845950325812</v>
+      </c>
+      <c r="R13" s="2">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="S13" s="3">
         <v>0.91576700913013875</v>
       </c>
-      <c r="O13" s="3">
+      <c r="T13" s="3">
         <v>0.40037216802098358</v>
       </c>
     </row>
-    <row r="14" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C14" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -5442,13 +5535,23 @@
         <v>9</v>
       </c>
       <c r="N14" s="3">
+        <v>0.91331446512726089</v>
+      </c>
+      <c r="O14" s="3">
+        <v>0.35478116543898081</v>
+      </c>
+      <c r="R14" s="2">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="S14" s="3">
         <v>0.91629778085011704</v>
       </c>
-      <c r="O14" s="3">
+      <c r="T14" s="3">
         <v>0.41710724468493471</v>
       </c>
     </row>
-    <row r="15" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C15" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -5474,13 +5577,23 @@
         <v>10</v>
       </c>
       <c r="N15" s="3">
+        <v>0.91072837877505441</v>
+      </c>
+      <c r="O15" s="3">
+        <v>0.43823305418082431</v>
+      </c>
+      <c r="R15" s="2">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="S15" s="3">
         <v>0.91531995687080647</v>
       </c>
-      <c r="O15" s="3">
+      <c r="T15" s="3">
         <v>0.40644823918019751</v>
       </c>
     </row>
-    <row r="16" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C16" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -5506,13 +5619,23 @@
         <v>11</v>
       </c>
       <c r="N16" s="3">
+        <v>0.91515257017113993</v>
+      </c>
+      <c r="O16" s="3">
+        <v>0.35184489365960803</v>
+      </c>
+      <c r="R16" s="2">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="S16" s="3">
         <v>0.91508993717462273</v>
       </c>
-      <c r="O16" s="3">
+      <c r="T16" s="3">
         <v>0.42371180495287841</v>
       </c>
     </row>
-    <row r="17" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C17" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -5538,13 +5661,23 @@
         <v>12</v>
       </c>
       <c r="N17" s="3">
+        <v>0.9107174539671461</v>
+      </c>
+      <c r="O17" s="3">
+        <v>0.36969333976529151</v>
+      </c>
+      <c r="R17" s="2">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="S17" s="3">
         <v>0.91701218012669916</v>
       </c>
-      <c r="O17" s="3">
+      <c r="T17" s="3">
         <v>0.35730168245153249</v>
       </c>
     </row>
-    <row r="18" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C18" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -5570,13 +5703,23 @@
         <v>13</v>
       </c>
       <c r="N18" s="3">
+        <v>0.91332542296532082</v>
+      </c>
+      <c r="O18" s="3">
+        <v>0.37948545332479527</v>
+      </c>
+      <c r="R18" s="2">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+      <c r="S18" s="3">
         <v>0.9169857547334499</v>
       </c>
-      <c r="O18" s="3">
+      <c r="T18" s="3">
         <v>0.37567610931786072</v>
       </c>
     </row>
-    <row r="19" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C19" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -5602,13 +5745,23 @@
         <v>14</v>
       </c>
       <c r="N19" s="3">
+        <v>0.9118783333899112</v>
+      </c>
+      <c r="O19" s="3">
+        <v>0.41645716616559331</v>
+      </c>
+      <c r="R19" s="2">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="S19" s="3">
         <v>0.9163667044504995</v>
       </c>
-      <c r="O19" s="3">
+      <c r="T19" s="3">
         <v>0.3499284852728487</v>
       </c>
     </row>
-    <row r="20" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C20" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -5634,13 +5787,23 @@
         <v>15</v>
       </c>
       <c r="N20" s="3">
+        <v>0.91221655045561056</v>
+      </c>
+      <c r="O20" s="3">
+        <v>0.41134613306511941</v>
+      </c>
+      <c r="R20" s="2">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="S20" s="3">
         <v>0.91554859111808162</v>
       </c>
-      <c r="O20" s="3">
+      <c r="T20" s="3">
         <v>0.38895611419692833</v>
       </c>
     </row>
-    <row r="21" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C21" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -5666,13 +5829,23 @@
         <v>16</v>
       </c>
       <c r="N21" s="3">
+        <v>0.91320835376654808</v>
+      </c>
+      <c r="O21" s="3">
+        <v>0.36877492449729993</v>
+      </c>
+      <c r="R21" s="2">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="S21" s="3">
         <v>0.91400113283412043</v>
       </c>
-      <c r="O21" s="3">
+      <c r="T21" s="3">
         <v>0.38858738304692808</v>
       </c>
     </row>
-    <row r="22" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C22" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -5698,13 +5871,23 @@
         <v>17</v>
       </c>
       <c r="N22" s="3">
+        <v>0.9104106798240168</v>
+      </c>
+      <c r="O22" s="3">
+        <v>0.36821008438198061</v>
+      </c>
+      <c r="R22" s="2">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+      <c r="S22" s="3">
         <v>0.91494649913581561</v>
       </c>
-      <c r="O22" s="3">
+      <c r="T22" s="3">
         <v>0.41813423426112328</v>
       </c>
     </row>
-    <row r="23" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C23" s="2">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -5730,13 +5913,23 @@
         <v>18</v>
       </c>
       <c r="N23" s="3">
+        <v>0.91320737359037529</v>
+      </c>
+      <c r="O23" s="3">
+        <v>0.39575510563990962</v>
+      </c>
+      <c r="R23" s="2">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+      <c r="S23" s="3">
         <v>0.91862013761439443</v>
       </c>
-      <c r="O23" s="3">
+      <c r="T23" s="3">
         <v>0.34851832729537569</v>
       </c>
     </row>
-    <row r="24" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C24" s="2">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -5762,13 +5955,23 @@
         <v>19</v>
       </c>
       <c r="N24" s="3">
+        <v>0.91441638665723113</v>
+      </c>
+      <c r="O24" s="3">
+        <v>0.38975932834371402</v>
+      </c>
+      <c r="R24" s="2">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+      <c r="S24" s="3">
         <v>0.91904839331541011</v>
       </c>
-      <c r="O24" s="3">
+      <c r="T24" s="3">
         <v>0.37308622757158549</v>
       </c>
     </row>
-    <row r="25" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C25" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -5794,13 +5997,23 @@
         <v>20</v>
       </c>
       <c r="N25" s="3">
+        <v>0.91248530527894034</v>
+      </c>
+      <c r="O25" s="3">
+        <v>0.41124739212079692</v>
+      </c>
+      <c r="R25" s="2">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="S25" s="3">
         <v>0.91594097757019866</v>
       </c>
-      <c r="O25" s="3">
+      <c r="T25" s="3">
         <v>0.38722401672688689</v>
       </c>
     </row>
-    <row r="26" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C26" s="2">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -5826,13 +6039,23 @@
         <v>21</v>
       </c>
       <c r="N26" s="3">
+        <v>0.91349203723346739</v>
+      </c>
+      <c r="O26" s="3">
+        <v>0.38425242765280071</v>
+      </c>
+      <c r="R26" s="2">
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
+      <c r="S26" s="3">
         <v>0.92005262613207539</v>
       </c>
-      <c r="O26" s="3">
+      <c r="T26" s="3">
         <v>0.38915628706909428</v>
       </c>
     </row>
-    <row r="27" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C27" s="2">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -5858,13 +6081,23 @@
         <v>22</v>
       </c>
       <c r="N27" s="3">
+        <v>0.91324254782579795</v>
+      </c>
+      <c r="O27" s="3">
+        <v>0.37917847069817401</v>
+      </c>
+      <c r="R27" s="2">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
+      <c r="S27" s="3">
         <v>0.91837667706163739</v>
       </c>
-      <c r="O27" s="3">
+      <c r="T27" s="3">
         <v>0.38469967380290437</v>
       </c>
     </row>
-    <row r="28" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C28" s="2">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -5890,13 +6123,23 @@
         <v>23</v>
       </c>
       <c r="N28" s="3">
+        <v>0.91672706062247722</v>
+      </c>
+      <c r="O28" s="3">
+        <v>0.33654793251971649</v>
+      </c>
+      <c r="R28" s="2">
+        <f t="shared" si="3"/>
+        <v>23</v>
+      </c>
+      <c r="S28" s="3">
         <v>0.91519590454594602</v>
       </c>
-      <c r="O28" s="3">
+      <c r="T28" s="3">
         <v>0.39888228116720859</v>
       </c>
     </row>
-    <row r="29" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C29" s="2">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -5922,13 +6165,23 @@
         <v>24</v>
       </c>
       <c r="N29" s="3">
+        <v>0.91328720489173421</v>
+      </c>
+      <c r="O29" s="3">
+        <v>0.38953730802563702</v>
+      </c>
+      <c r="R29" s="2">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="S29" s="3">
         <v>0.91764578331319779</v>
       </c>
-      <c r="O29" s="3">
+      <c r="T29" s="3">
         <v>0.36131962232278469</v>
       </c>
     </row>
-    <row r="30" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C30" s="2">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -5954,13 +6207,23 @@
         <v>25</v>
       </c>
       <c r="N30" s="3">
+        <v>0.91466662691974054</v>
+      </c>
+      <c r="O30" s="3">
+        <v>0.35000069471261669</v>
+      </c>
+      <c r="R30" s="2">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+      <c r="S30" s="3">
         <v>0.91596873400574697</v>
       </c>
-      <c r="O30" s="3">
+      <c r="T30" s="3">
         <v>0.39691588478809248</v>
       </c>
     </row>
-    <row r="31" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C31" s="2">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -5986,13 +6249,23 @@
         <v>26</v>
       </c>
       <c r="N31" s="3">
+        <v>0.91045396727293815</v>
+      </c>
+      <c r="O31" s="3">
+        <v>0.39495590401929748</v>
+      </c>
+      <c r="R31" s="2">
+        <f t="shared" si="3"/>
+        <v>26</v>
+      </c>
+      <c r="S31" s="3">
         <v>0.91641544032332634</v>
       </c>
-      <c r="O31" s="3">
+      <c r="T31" s="3">
         <v>0.39881906517000559</v>
       </c>
     </row>
-    <row r="32" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C32" s="2">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -6018,13 +6291,23 @@
         <v>27</v>
       </c>
       <c r="N32" s="3">
+        <v>0.91347914720835921</v>
+      </c>
+      <c r="O32" s="3">
+        <v>0.38246809102345602</v>
+      </c>
+      <c r="R32" s="2">
+        <f t="shared" si="3"/>
+        <v>27</v>
+      </c>
+      <c r="S32" s="3">
         <v>0.91718401128277638</v>
       </c>
-      <c r="O32" s="3">
+      <c r="T32" s="3">
         <v>0.38697986038763471</v>
       </c>
     </row>
-    <row r="33" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C33" s="2">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -6050,13 +6333,23 @@
         <v>28</v>
       </c>
       <c r="N33" s="3">
+        <v>0.91284025307522432</v>
+      </c>
+      <c r="O33" s="3">
+        <v>0.37354528691628691</v>
+      </c>
+      <c r="R33" s="2">
+        <f t="shared" si="3"/>
+        <v>28</v>
+      </c>
+      <c r="S33" s="3">
         <v>0.91431860944516252</v>
       </c>
-      <c r="O33" s="3">
+      <c r="T33" s="3">
         <v>0.41001950594048059</v>
       </c>
     </row>
-    <row r="34" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C34" s="2">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -6082,13 +6375,23 @@
         <v>29</v>
       </c>
       <c r="N34" s="3">
+        <v>0.91320184810291682</v>
+      </c>
+      <c r="O34" s="3">
+        <v>0.33897102033577448</v>
+      </c>
+      <c r="R34" s="2">
+        <f t="shared" si="3"/>
+        <v>29</v>
+      </c>
+      <c r="S34" s="3">
         <v>0.91402482133323393</v>
       </c>
-      <c r="O34" s="3">
+      <c r="T34" s="3">
         <v>0.39437206374319189</v>
       </c>
     </row>
-    <row r="35" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C35" s="2">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -6114,13 +6417,23 @@
         <v>30</v>
       </c>
       <c r="N35" s="3">
+        <v>0.91469191366183999</v>
+      </c>
+      <c r="O35" s="3">
+        <v>0.34821879903991082</v>
+      </c>
+      <c r="R35" s="2">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+      <c r="S35" s="3">
         <v>0.91467658667899387</v>
       </c>
-      <c r="O35" s="3">
+      <c r="T35" s="3">
         <v>0.4454616877559745</v>
       </c>
     </row>
-    <row r="36" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C36" s="2">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -6146,13 +6459,23 @@
         <v>31</v>
       </c>
       <c r="N36" s="3">
+        <v>0.9121370183548152</v>
+      </c>
+      <c r="O36" s="3">
+        <v>0.37886094659264441</v>
+      </c>
+      <c r="R36" s="2">
+        <f t="shared" si="3"/>
+        <v>31</v>
+      </c>
+      <c r="S36" s="3">
         <v>0.91377918955119264</v>
       </c>
-      <c r="O36" s="3">
+      <c r="T36" s="3">
         <v>0.44003922301779042</v>
       </c>
     </row>
-    <row r="37" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C37" s="2">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -6178,13 +6501,23 @@
         <v>32</v>
       </c>
       <c r="N37" s="3">
+        <v>0.9093318006702199</v>
+      </c>
+      <c r="O37" s="3">
+        <v>0.45233962134035338</v>
+      </c>
+      <c r="R37" s="2">
+        <f t="shared" si="3"/>
+        <v>32</v>
+      </c>
+      <c r="S37" s="3">
         <v>0.91463797687703963</v>
       </c>
-      <c r="O37" s="3">
+      <c r="T37" s="3">
         <v>0.39341116856419422</v>
       </c>
     </row>
-    <row r="38" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C38" s="2">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -6210,13 +6543,23 @@
         <v>33</v>
       </c>
       <c r="N38" s="3">
+        <v>0.91200567987169112</v>
+      </c>
+      <c r="O38" s="3">
+        <v>0.36603230318934721</v>
+      </c>
+      <c r="R38" s="2">
+        <f t="shared" si="3"/>
+        <v>33</v>
+      </c>
+      <c r="S38" s="3">
         <v>0.9172809112516408</v>
       </c>
-      <c r="O38" s="3">
+      <c r="T38" s="3">
         <v>0.34003429378544819</v>
       </c>
     </row>
-    <row r="39" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C39" s="2">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -6242,13 +6585,23 @@
         <v>34</v>
       </c>
       <c r="N39" s="3">
+        <v>0.913070630731323</v>
+      </c>
+      <c r="O39" s="3">
+        <v>0.39009480154484572</v>
+      </c>
+      <c r="R39" s="2">
+        <f t="shared" si="3"/>
+        <v>34</v>
+      </c>
+      <c r="S39" s="3">
         <v>0.91567609942069617</v>
       </c>
-      <c r="O39" s="3">
+      <c r="T39" s="3">
         <v>0.37609375561764952</v>
       </c>
     </row>
-    <row r="40" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C40" s="2">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -6274,13 +6627,23 @@
         <v>35</v>
       </c>
       <c r="N40" s="3">
+        <v>0.91262390636704538</v>
+      </c>
+      <c r="O40" s="3">
+        <v>0.36933683844086002</v>
+      </c>
+      <c r="R40" s="2">
+        <f t="shared" si="3"/>
+        <v>35</v>
+      </c>
+      <c r="S40" s="3">
         <v>0.91449227287901691</v>
       </c>
-      <c r="O40" s="3">
+      <c r="T40" s="3">
         <v>0.40884290123165667</v>
       </c>
     </row>
-    <row r="41" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C41" s="2">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -6306,13 +6669,23 @@
         <v>36</v>
       </c>
       <c r="N41" s="3">
+        <v>0.91344464264080683</v>
+      </c>
+      <c r="O41" s="3">
+        <v>0.39295478340743639</v>
+      </c>
+      <c r="R41" s="2">
+        <f t="shared" si="3"/>
+        <v>36</v>
+      </c>
+      <c r="S41" s="3">
         <v>0.91416950909439165</v>
       </c>
-      <c r="O41" s="3">
+      <c r="T41" s="3">
         <v>0.39484564368256192</v>
       </c>
     </row>
-    <row r="42" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C42" s="2">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -6338,13 +6711,23 @@
         <v>37</v>
       </c>
       <c r="N42" s="3">
+        <v>0.91133853722957303</v>
+      </c>
+      <c r="O42" s="3">
+        <v>0.35754300358478491</v>
+      </c>
+      <c r="R42" s="2">
+        <f t="shared" si="3"/>
+        <v>37</v>
+      </c>
+      <c r="S42" s="3">
         <v>0.91536719185468263</v>
       </c>
-      <c r="O42" s="3">
+      <c r="T42" s="3">
         <v>0.4405499570392416</v>
       </c>
     </row>
-    <row r="43" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C43" s="2">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -6370,13 +6753,23 @@
         <v>38</v>
       </c>
       <c r="N43" s="3">
+        <v>0.91190319841790757</v>
+      </c>
+      <c r="O43" s="3">
+        <v>0.40342004022803579</v>
+      </c>
+      <c r="R43" s="2">
+        <f t="shared" si="3"/>
+        <v>38</v>
+      </c>
+      <c r="S43" s="3">
         <v>0.91576897088313913</v>
       </c>
-      <c r="O43" s="3">
+      <c r="T43" s="3">
         <v>0.3687152609541301</v>
       </c>
     </row>
-    <row r="44" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C44" s="2">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -6402,13 +6795,23 @@
         <v>39</v>
       </c>
       <c r="N44" s="3">
+        <v>0.91216829167592661</v>
+      </c>
+      <c r="O44" s="3">
+        <v>0.42781261266331783</v>
+      </c>
+      <c r="R44" s="2">
+        <f t="shared" si="3"/>
+        <v>39</v>
+      </c>
+      <c r="S44" s="3">
         <v>0.9147998660208444</v>
       </c>
-      <c r="O44" s="3">
+      <c r="T44" s="3">
         <v>0.40257104356507312</v>
       </c>
     </row>
-    <row r="45" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C45" s="2">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -6434,13 +6837,23 @@
         <v>40</v>
       </c>
       <c r="N45" s="3">
+        <v>0.91354548745440256</v>
+      </c>
+      <c r="O45" s="3">
+        <v>0.38338699551935029</v>
+      </c>
+      <c r="R45" s="2">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+      <c r="S45" s="3">
         <v>0.91424161135204685</v>
       </c>
-      <c r="O45" s="3">
+      <c r="T45" s="3">
         <v>0.41426389125770458</v>
       </c>
     </row>
-    <row r="46" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C46" s="2">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -6466,13 +6879,23 @@
         <v>41</v>
       </c>
       <c r="N46" s="3">
+        <v>0.91302586371375272</v>
+      </c>
+      <c r="O46" s="3">
+        <v>0.41846506182558368</v>
+      </c>
+      <c r="R46" s="2">
+        <f t="shared" si="3"/>
+        <v>41</v>
+      </c>
+      <c r="S46" s="3">
         <v>0.91408621853011629</v>
       </c>
-      <c r="O46" s="3">
+      <c r="T46" s="3">
         <v>0.44162951455098748</v>
       </c>
     </row>
-    <row r="47" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C47" s="2">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -6498,13 +6921,23 @@
         <v>42</v>
       </c>
       <c r="N47" s="3">
+        <v>0.91379630520861532</v>
+      </c>
+      <c r="O47" s="3">
+        <v>0.3719622314227844</v>
+      </c>
+      <c r="R47" s="2">
+        <f t="shared" si="3"/>
+        <v>42</v>
+      </c>
+      <c r="S47" s="3">
         <v>0.91410209538498743</v>
       </c>
-      <c r="O47" s="3">
+      <c r="T47" s="3">
         <v>0.40804586444538848</v>
       </c>
     </row>
-    <row r="48" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C48" s="2">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -6530,13 +6963,23 @@
         <v>43</v>
       </c>
       <c r="N48" s="3">
+        <v>0.91194140643331167</v>
+      </c>
+      <c r="O48" s="3">
+        <v>0.37904447506022582</v>
+      </c>
+      <c r="R48" s="2">
+        <f t="shared" si="3"/>
+        <v>43</v>
+      </c>
+      <c r="S48" s="3">
         <v>0.91586147783740102</v>
       </c>
-      <c r="O48" s="3">
+      <c r="T48" s="3">
         <v>0.39836986921977269</v>
       </c>
     </row>
-    <row r="49" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C49" s="2">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -6562,13 +7005,23 @@
         <v>44</v>
       </c>
       <c r="N49" s="3">
+        <v>0.91357259441659755</v>
+      </c>
+      <c r="O49" s="3">
+        <v>0.3923925238443412</v>
+      </c>
+      <c r="R49" s="2">
+        <f t="shared" si="3"/>
+        <v>44</v>
+      </c>
+      <c r="S49" s="3">
         <v>0.91677789000881449</v>
       </c>
-      <c r="O49" s="3">
+      <c r="T49" s="3">
         <v>0.39996472523342508</v>
       </c>
     </row>
-    <row r="50" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C50" s="2">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -6594,13 +7047,23 @@
         <v>45</v>
       </c>
       <c r="N50" s="3">
+        <v>0.91379950960577072</v>
+      </c>
+      <c r="O50" s="3">
+        <v>0.3786837675898248</v>
+      </c>
+      <c r="R50" s="2">
+        <f t="shared" si="3"/>
+        <v>45</v>
+      </c>
+      <c r="S50" s="3">
         <v>0.91708593158818164</v>
       </c>
-      <c r="O50" s="3">
+      <c r="T50" s="3">
         <v>0.38912587901636991</v>
       </c>
     </row>
-    <row r="51" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C51" s="2">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -6626,13 +7089,23 @@
         <v>46</v>
       </c>
       <c r="N51" s="3">
+        <v>0.91306805724144591</v>
+      </c>
+      <c r="O51" s="3">
+        <v>0.40643717131231077</v>
+      </c>
+      <c r="R51" s="2">
+        <f t="shared" si="3"/>
+        <v>46</v>
+      </c>
+      <c r="S51" s="3">
         <v>0.91625575276340765</v>
       </c>
-      <c r="O51" s="3">
+      <c r="T51" s="3">
         <v>0.44732877335927668</v>
       </c>
     </row>
-    <row r="52" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C52" s="2">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -6658,13 +7131,23 @@
         <v>47</v>
       </c>
       <c r="N52" s="3">
+        <v>0.91192090172372231</v>
+      </c>
+      <c r="O52" s="3">
+        <v>0.41428238640324833</v>
+      </c>
+      <c r="R52" s="2">
+        <f t="shared" si="3"/>
+        <v>47</v>
+      </c>
+      <c r="S52" s="3">
         <v>0.91852446230503537</v>
       </c>
-      <c r="O52" s="3">
+      <c r="T52" s="3">
         <v>0.3380688335154195</v>
       </c>
     </row>
-    <row r="53" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C53" s="2">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -6690,13 +7173,23 @@
         <v>48</v>
       </c>
       <c r="N53" s="3">
+        <v>0.91090990794508386</v>
+      </c>
+      <c r="O53" s="3">
+        <v>0.3925097258139274</v>
+      </c>
+      <c r="R53" s="2">
+        <f t="shared" si="3"/>
+        <v>48</v>
+      </c>
+      <c r="S53" s="3">
         <v>0.91486079051840807</v>
       </c>
-      <c r="O53" s="3">
+      <c r="T53" s="3">
         <v>0.43483910889518212</v>
       </c>
     </row>
-    <row r="54" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C54" s="2">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -6722,13 +7215,23 @@
         <v>49</v>
       </c>
       <c r="N54" s="3">
+        <v>0.91245183847036637</v>
+      </c>
+      <c r="O54" s="3">
+        <v>0.37183555755799658</v>
+      </c>
+      <c r="R54" s="2">
+        <f t="shared" si="3"/>
+        <v>49</v>
+      </c>
+      <c r="S54" s="3">
         <v>0.91394752193381767</v>
       </c>
-      <c r="O54" s="3">
+      <c r="T54" s="3">
         <v>0.42935014232565699</v>
       </c>
     </row>
-    <row r="55" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C55" s="2">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -6754,13 +7257,23 @@
         <v>50</v>
       </c>
       <c r="N55" s="3">
+        <v>0.91252176494777926</v>
+      </c>
+      <c r="O55" s="3">
+        <v>0.39203177813006512</v>
+      </c>
+      <c r="R55" s="2">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="S55" s="3">
         <v>0.91717594991159113</v>
       </c>
-      <c r="O55" s="3">
+      <c r="T55" s="3">
         <v>0.41452494778909632</v>
       </c>
     </row>
-    <row r="57" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C57" s="2" t="s">
         <v>3</v>
       </c>
@@ -6788,14 +7301,25 @@
       </c>
       <c r="N57" s="3">
         <f>AVERAGE(N6:N55)</f>
-        <v>0.91580572419307349</v>
+        <v>0.91279702532560436</v>
       </c>
       <c r="O57" s="3">
         <f>AVERAGE(O6:O55)</f>
+        <v>0.38291683774093449</v>
+      </c>
+      <c r="R57" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="S57" s="3">
+        <f>AVERAGE(S6:S55)</f>
+        <v>0.91580572419307349</v>
+      </c>
+      <c r="T57" s="3">
+        <f>AVERAGE(T6:T55)</f>
         <v>0.3996071039119895</v>
       </c>
     </row>
-    <row r="58" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C58" s="2" t="s">
         <v>4</v>
       </c>
@@ -6823,10 +7347,21 @@
       </c>
       <c r="N58" s="3">
         <f>_xlfn.STDEV.S(N6:N55)</f>
-        <v>1.5188559427630813E-3</v>
+        <v>1.6236559627426552E-3</v>
       </c>
       <c r="O58" s="3">
         <f>_xlfn.STDEV.S(O6:O55)</f>
+        <v>2.9620820845424164E-2</v>
+      </c>
+      <c r="R58" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="S58" s="3">
+        <f>_xlfn.STDEV.S(S6:S55)</f>
+        <v>1.5188559427630813E-3</v>
+      </c>
+      <c r="T58" s="3">
+        <f>_xlfn.STDEV.S(T6:T55)</f>
         <v>2.681351017293333E-2</v>
       </c>
     </row>

</xml_diff>